<commit_message>
fix carga masiva usuarios
</commit_message>
<xml_diff>
--- a/src/assets/files/13.Personal.xlsx
+++ b/src/assets/files/13.Personal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brquezada\Documents\projects\frontEnd\gui-mst-adt-web\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB62BD5-EA3D-4F51-942F-E85DD928F4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BF0C72-2C14-4755-8E7F-8A582660DDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{B2AA2D53-D174-4EA3-914E-515F0616B07E}"/>
+    <workbookView xWindow="-16560" yWindow="-3274" windowWidth="16663" windowHeight="9017" activeTab="3" xr2:uid="{B2AA2D53-D174-4EA3-914E-515F0616B07E}"/>
   </bookViews>
   <sheets>
     <sheet name="Z_roles" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t xml:space="preserve">Administrador </t>
   </si>
@@ -49,15 +49,6 @@
     <t>Jefe_trabajo_social</t>
   </si>
   <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>NOMBRE COMPLETO</t>
-  </si>
-  <si>
     <t>PUESTO</t>
   </si>
   <si>
@@ -70,12 +61,6 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>SEGUNDO APELLIDO</t>
-  </si>
-  <si>
-    <t>PRIMER APELLIDO</t>
-  </si>
-  <si>
     <t>TURNO</t>
   </si>
   <si>
@@ -103,17 +88,38 @@
     <t>Carlos</t>
   </si>
   <si>
-    <t>Carlos Salas Perez</t>
-  </si>
-  <si>
-    <t>cperez</t>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>UNIDAD_MEDICA</t>
+  </si>
+  <si>
+    <t>HGSMF8</t>
+  </si>
+  <si>
+    <t>ESCUELA_PROCEDENCIA</t>
+  </si>
+  <si>
+    <t>fulanito@gmail.com</t>
+  </si>
+  <si>
+    <t>UAT</t>
+  </si>
+  <si>
+    <t>CONTRASEÑA</t>
+  </si>
+  <si>
+    <t>PRIMER_APELLIDO</t>
+  </si>
+  <si>
+    <t>SEGUNDO_APELLIDO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +132,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,10 +159,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -160,8 +175,10 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,17 +497,17 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -508,14 +525,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -533,46 +550,46 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F23" s="4"/>
     </row>
   </sheetData>
@@ -583,59 +600,65 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DA98A0-E158-48D8-9C97-9AF22F5D5CB8}">
-  <dimension ref="A1:K103"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="6" width="14.08984375" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
       <c r="I1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>987654321</v>
@@ -646,20 +669,23 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>987654321</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2">
-        <v>987654321</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -667,362 +693,15 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G46" t="str">
-        <f t="shared" ref="G46:G77" si="0">CONCATENATE(A46," ",B46," ",C46)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G47" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G48" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G49" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G50" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G51" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G52" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G53" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G54" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G55" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G56" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G57" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G58" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G59" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G60" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G61" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G62" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G63" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G64" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G65" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G66" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G67" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G68" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G69" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G70" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G71" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G72" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G73" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G74" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G75" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G76" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G77" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G78" t="str">
-        <f t="shared" ref="G78:G103" si="1">CONCATENATE(A78," ",B78," ",C78)</f>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G79" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G80" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G81" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G82" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G83" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G84" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G85" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G86" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G87" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G88" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G89" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G90" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G91" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G92" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G93" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G94" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G95" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G96" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G97" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G98" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G99" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G100" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G101" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G102" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G103" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  </v>
-      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{51981917-877C-4216-952E-BCE21AECEBB1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1039,21 +718,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002047D94B5E73D04A80AA6844A59F543A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="19f8b377e75dbac3c1f2314aec064948">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f6edc329ff236629c56e3b879b320d0">
     <xsd:element name="properties">
@@ -1167,24 +831,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38A4FBA4-4667-40CF-86DF-E36A46A91476}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC525CC-64EB-4964-A86D-BD5ECA102CAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E1B4948-F3FE-4007-A8E4-B0A2ED3DBCEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1198,4 +860,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC525CC-64EB-4964-A86D-BD5ECA102CAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38A4FBA4-4667-40CF-86DF-E36A46A91476}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix cargas masivas usuarios, turnos y puestos
</commit_message>
<xml_diff>
--- a/src/assets/files/13.Personal.xlsx
+++ b/src/assets/files/13.Personal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\validacionesUsuarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA6527A-3B7A-452D-9518-8B7195578E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE39EF48-424E-4458-9838-85C52B5E9742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="684" windowWidth="16440" windowHeight="8928" activeTab="3" xr2:uid="{B2AA2D53-D174-4EA3-914E-515F0616B07E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="8983" activeTab="3" xr2:uid="{B2AA2D53-D174-4EA3-914E-515F0616B07E}"/>
   </bookViews>
   <sheets>
     <sheet name="Z_roles" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
   <si>
     <t>Asistente</t>
   </si>
@@ -55,12 +55,6 @@
     <t xml:space="preserve">Administrador </t>
   </si>
   <si>
-    <t>Alfabético</t>
-  </si>
-  <si>
-    <t>Not null</t>
-  </si>
-  <si>
     <t>DESCRIPCION</t>
   </si>
   <si>
@@ -97,36 +91,15 @@
     <t>Auxiliar</t>
   </si>
   <si>
-    <t>Para la carga de personal se requiere tener precargados los roles en el sistema</t>
-  </si>
-  <si>
-    <t>Para la carga de personal se requiere tener precargados los puestos en el sistema</t>
-  </si>
-  <si>
-    <t>Primaria</t>
-  </si>
-  <si>
     <t>TURNO</t>
   </si>
   <si>
-    <t>Clave turno</t>
-  </si>
-  <si>
     <t>Descripción de turno</t>
   </si>
   <si>
     <t>4_30_6</t>
   </si>
   <si>
-    <t>not null</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>numérico</t>
-  </si>
-  <si>
     <t>No especificado</t>
   </si>
   <si>
@@ -262,9 +235,6 @@
     <t xml:space="preserve">Vazquez </t>
   </si>
   <si>
-    <t>CONTRASEÑA</t>
-  </si>
-  <si>
     <t>EMAIL</t>
   </si>
   <si>
@@ -274,9 +244,6 @@
     <t>valentina.delarosa@imss.gob.mx</t>
   </si>
   <si>
-    <t>martine.acosta@@imss.gob.mx</t>
-  </si>
-  <si>
     <t>juanf.delcorral@imss.gob.mx</t>
   </si>
   <si>
@@ -298,6 +265,9 @@
     <t>rebeca.casas@imss.gob.mx</t>
   </si>
   <si>
+    <t>ESCUELA_PROCEDENCIA</t>
+  </si>
+  <si>
     <t>PRIMER_APELLIDO</t>
   </si>
   <si>
@@ -317,13 +287,16 @@
   </si>
   <si>
     <t>efrain.vazquez@imss.gob.mx</t>
+  </si>
+  <si>
+    <t>martine.acosta@imss.gob.mx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,12 +317,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -373,16 +340,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -698,65 +662,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457DE737-224B-4933-96EB-24C7FA63A79C}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -766,62 +715,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEA07F1-85A9-4A44-B79B-F6F66A073F2B}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.85">
+      <c r="A7" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -831,123 +765,75 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201BC9CC-04B5-4017-B56F-66113710697B}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.421875" defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.85">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.85">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.85">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.85">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.85">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.85">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F23" s="2"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.85">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.85">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.85">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.85">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.85">
+      <c r="E20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -960,54 +846,56 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
   <cols>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" customWidth="1"/>
+    <col min="5" max="5" width="14.11328125" customWidth="1"/>
+    <col min="6" max="6" width="23.8828125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.65234375" customWidth="1"/>
+    <col min="9" max="9" width="21.421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>74</v>
-      </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>912083456</v>
@@ -1016,27 +904,24 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>912083456</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>975432729</v>
@@ -1045,56 +930,50 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3">
-        <v>975432729</v>
-      </c>
-      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.85">
+      <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>123453894</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4">
-        <v>123453894</v>
-      </c>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>974348722</v>
@@ -1103,27 +982,24 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>974348722</v>
-      </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>864263789</v>
@@ -1132,27 +1008,24 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>864263789</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D7">
         <v>534283945</v>
@@ -1161,27 +1034,24 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7">
-        <v>534283945</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>834417268</v>
@@ -1190,27 +1060,24 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8">
-        <v>834417268</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>723498109</v>
@@ -1219,27 +1086,24 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>723498109</v>
-      </c>
-      <c r="H9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D10">
         <v>987938743</v>
@@ -1248,27 +1112,24 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>987938743</v>
-      </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D11">
         <v>872345903</v>
@@ -1277,56 +1138,50 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11">
-        <v>872345903</v>
-      </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>876234879</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12">
-        <v>876234879</v>
-      </c>
-      <c r="H12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D13">
         <v>123257965</v>
@@ -1335,27 +1190,24 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13">
-        <v>123257965</v>
-      </c>
-      <c r="H13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.85">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D14">
         <v>99091173</v>
@@ -1364,42 +1216,40 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14">
-        <v>99091173</v>
-      </c>
-      <c r="H14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>88</v>
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{7ACCB081-B991-41C3-843D-D19D0AA3A325}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{F3DCFE94-2834-4929-8222-2A56D3EC790B}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{2C6420DA-9EB6-4B6F-9A57-A891074D94F0}"/>
-    <hyperlink ref="I6" r:id="rId4" xr:uid="{36356BA0-092E-4E03-A9D7-EFCBE323993F}"/>
-    <hyperlink ref="I7" r:id="rId5" xr:uid="{A87E6306-7004-48D1-9F0D-C0E93813AFF2}"/>
-    <hyperlink ref="I8" r:id="rId6" xr:uid="{9FBBA67F-3B04-460E-B74C-0EE192987D7E}"/>
-    <hyperlink ref="I9" r:id="rId7" xr:uid="{E25B3C92-1B8C-4543-A83A-958F0E6E1DB8}"/>
-    <hyperlink ref="I10" r:id="rId8" xr:uid="{D86D5EE9-BD49-4F57-8A9A-0A37D9C7A302}"/>
-    <hyperlink ref="I11" r:id="rId9" xr:uid="{13CC5EAA-E452-4BD6-8FFD-7A66A42FEF14}"/>
-    <hyperlink ref="I12" r:id="rId10" xr:uid="{C91638C3-42BA-4D11-810A-29EE49B14F4E}"/>
-    <hyperlink ref="I13" r:id="rId11" xr:uid="{7E5CBDDB-1038-41D9-958B-EFA878D4A97D}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{7ACCB081-B991-41C3-843D-D19D0AA3A325}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{F3DCFE94-2834-4929-8222-2A56D3EC790B}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{2C6420DA-9EB6-4B6F-9A57-A891074D94F0}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{36356BA0-092E-4E03-A9D7-EFCBE323993F}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{A87E6306-7004-48D1-9F0D-C0E93813AFF2}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{9FBBA67F-3B04-460E-B74C-0EE192987D7E}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{E25B3C92-1B8C-4543-A83A-958F0E6E1DB8}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{D86D5EE9-BD49-4F57-8A9A-0A37D9C7A302}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{13CC5EAA-E452-4BD6-8FFD-7A66A42FEF14}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{C91638C3-42BA-4D11-810A-29EE49B14F4E}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{7E5CBDDB-1038-41D9-958B-EFA878D4A97D}"/>
+    <hyperlink ref="H5" r:id="rId12" xr:uid="{3D9A04F7-B018-434A-A948-7D45C8D5E9FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{631D863E-8BE5-489D-869C-F96E25C4338A}">
           <x14:formula1>
-            <xm:f>Z_roles!$A$5:$A$23</xm:f>
+            <xm:f>Z_roles!$A$2:$A$20</xm:f>
           </x14:formula1>
-          <xm:sqref>E52:H93</xm:sqref>
+          <xm:sqref>E52:G93</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>